<commit_message>
adding vessel numbers to igraph object
</commit_message>
<xml_diff>
--- a/data/input/species_groupings IEA.xlsx
+++ b/data/input/species_groupings IEA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameal.samhouri/Dropbox/CCIEA/cciea_networks_git/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A048877-4947-8742-9393-C684A1575357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5A1BAA-EBB1-8E4A-9624-55B043EA3C4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22220" yWindow="2620" windowWidth="27320" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20880" yWindow="2600" windowWidth="27320" windowHeight="20140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SPID_SPGRPM" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="727">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="745">
   <si>
     <t>SPID</t>
   </si>
@@ -2209,6 +2209,60 @@
   </si>
   <si>
     <t>PBTR</t>
+  </si>
+  <si>
+    <t>species_group_2_label2</t>
+  </si>
+  <si>
+    <t>DTS groundfish</t>
+  </si>
+  <si>
+    <t>Whiting</t>
+  </si>
+  <si>
+    <t>Non-DTS groundfish</t>
+  </si>
+  <si>
+    <t>Skate/dogfish/shark</t>
+  </si>
+  <si>
+    <t>Prawns/shrimp</t>
+  </si>
+  <si>
+    <t>Pink shrimp</t>
+  </si>
+  <si>
+    <t>Crab</t>
+  </si>
+  <si>
+    <t>Salmon</t>
+  </si>
+  <si>
+    <t>Tuna</t>
+  </si>
+  <si>
+    <t>Herring</t>
+  </si>
+  <si>
+    <t>Coastal pelagics</t>
+  </si>
+  <si>
+    <t>Pacific halibut</t>
+  </si>
+  <si>
+    <t>CA halibut/croaker</t>
+  </si>
+  <si>
+    <t>Echinoderms</t>
+  </si>
+  <si>
+    <t>Shellfish</t>
+  </si>
+  <si>
+    <t>Squid</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -2528,8 +2582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A10:G358"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A339" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O350" sqref="O350"/>
+    <sheetView topLeftCell="A235" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B250" sqref="B250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10425,159 +10479,213 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection sqref="A1:B31"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C18" sqref="C1:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>681</v>
       </c>
       <c r="B1" t="s">
         <v>682</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>686</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>687</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>25</v>
       </c>
       <c r="B8" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>690</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>35</v>
       </c>
       <c r="B10" t="s">
         <v>691</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>40</v>
       </c>
       <c r="B11" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>45</v>
       </c>
       <c r="B12" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>50</v>
       </c>
       <c r="B13" t="s">
         <v>694</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>55</v>
       </c>
       <c r="B14" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>60</v>
       </c>
       <c r="B15" t="s">
         <v>696</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>65</v>
       </c>
       <c r="B16" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>70</v>
       </c>
       <c r="B17" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>80</v>
       </c>
       <c r="B18" t="s">
         <v>699</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>100</v>
       </c>
@@ -10585,7 +10693,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>110</v>
       </c>
@@ -10593,7 +10701,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>118</v>
       </c>
@@ -10601,7 +10709,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>139</v>
       </c>
@@ -10609,7 +10717,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>193</v>
       </c>
@@ -10617,7 +10725,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>200</v>
       </c>
@@ -10625,7 +10733,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>230</v>
       </c>
@@ -10633,7 +10741,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>270</v>
       </c>
@@ -10641,7 +10749,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>400</v>
       </c>
@@ -10649,7 +10757,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>710</v>
       </c>
@@ -10657,7 +10765,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>800</v>
       </c>
@@ -10665,7 +10773,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>815</v>
       </c>
@@ -10673,7 +10781,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>900</v>
       </c>

</xml_diff>